<commit_message>
all pricings and features are now read from csv
</commit_message>
<xml_diff>
--- a/provs/google/historical data google.xlsx
+++ b/provs/google/historical data google.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="18915" windowHeight="11250" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="18915" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="ondemand" sheetId="2" r:id="rId1"/>
@@ -134,10 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
-  <si>
-    <t>Keyword</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>Provider</t>
   </si>
@@ -239,6 +236,12 @@
   </si>
   <si>
     <t>us-central2-a</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -640,119 +643,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>20120628</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>25</v>
+      <c r="B2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>20120628</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>26</v>
+      <c r="B3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>20120628</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>27</v>
+      <c r="B4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>20120628</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
+      <c r="B5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +785,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,60 +809,60 @@
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="E2" s="4">
         <v>3.75</v>
@@ -870,16 +889,16 @@
     </row>
     <row r="3" spans="1:14" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="E3" s="4">
         <v>7.5</v>
@@ -906,16 +925,16 @@
     </row>
     <row r="4" spans="1:14" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="E4" s="4">
         <v>15</v>
@@ -942,16 +961,16 @@
     </row>
     <row r="5" spans="1:14" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="E5" s="4">
         <v>30</v>
@@ -988,9 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -999,45 +1016,45 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="I1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="4">
         <v>3.75</v>
@@ -1059,13 +1076,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="4">
         <v>7.5</v>
@@ -1087,13 +1104,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="4">
         <v>15</v>
@@ -1115,13 +1132,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D5" s="4">
         <v>30</v>

</xml_diff>